<commit_message>
made changes to program
</commit_message>
<xml_diff>
--- a/module_info.xlsx
+++ b/module_info.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chowshengyang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chowshengyang/Documents/GitHub/streamlit-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76784FE2-D81B-A749-95FB-7236C1EE20D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1257AA7-E541-FD48-8871-76215CB0EB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{E06FD485-DB9E-E648-94D6-64559FF2D8D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$938</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1784,7 +1787,7 @@
   <dimension ref="A1:D938"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -9656,6 +9659,7 @@
       <c r="D938" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D938" xr:uid="{7403A18C-78F2-A943-B04C-BFC48D7F7149}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>